<commit_message>
chore: Update script and storyboard according to review's feedback.
</commit_message>
<xml_diff>
--- a/The Protagonist's Journey - Script.xlsx
+++ b/The Protagonist's Journey - Script.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
   <si>
     <t>TITLE</t>
   </si>
@@ -52,16 +52,19 @@
     <t xml:space="preserve">OTHER COMMENTS </t>
   </si>
   <si>
-    <t>Camera system is placed in San Martín square at an equal distance between the Cathedral, Cabildo and San Martín monument. At this location the "meet up" between the tour guide and the visitor happen at 10am.</t>
+    <t xml:space="preserve">Camera system is placed in San Martín square at an equal distance between the Cathedral, Cabildo and San Martín monument. At this location the "meet up" between the tour guide and the visitor happen at 10am. It is a partially clouded day. At this time of the day the lightning is optimal. It is getting colded due to the time of the year (almost winter) so both the guide and visitor are wearing jackets. </t>
   </si>
   <si>
     <t>People from Córdoba is passing by since this a touristic point in the city.</t>
   </si>
   <si>
-    <t xml:space="preserve">VISITOR (V): Hi, my name is Pablo, we spoke on the phone about the tour though "Centro Histórico". </t>
+    <t>SCENE 1</t>
   </si>
   <si>
-    <t xml:space="preserve">It's 10am. Pablo is waiting for the tour guide to arrive at the arranged location. At the exact time, the tour guide arrives to the meeting point. The tour guide is a lady and she has a badge hanging in her jacket it is really easy for the visitor to know she was the person he was expecting. </t>
+    <t xml:space="preserve">It's 10am. Pablo is waiting for the tour guide to arrive at the arranged location. At the exact time, the tour guide appears from behind Cabildo and walks towards the meeting point. Her name is Marisa and she has a badge hanging in her jacket so it is really easy for the visitor to know she was the person he was expecting. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISITOR (V): Hi, my name is Pablo, we spoke on the phone about the tour though "Centro Histórico". </t>
   </si>
   <si>
     <t xml:space="preserve">TOUR GUIDE (TG): HI, my name is Marisa. We spoke on the phone a few days ago. Nice to meet you. </t>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">TG: Sure, we will start at this location which is San Martín Square, we will revisit historical points about it, then we will go to the Cathedral which is right next to us and there we will talk about its history, the architecture and will know the interior and the different chapels in it. Once we leave the cathedral we will then move to Cabildo (city hall) and will see how this place was during colonial times. We will visit patio mayor (where the governor lived during the mentioned period), patio menor, its recent discoveries and the first and former prision also located inside Cabildo. Once we completed this tour we will wrap up the interview in the main entrance and we will briefly talk about the recent updates we had from local artists </t>
   </si>
   <si>
+    <t>A mother and her daugther passes behind us and they cannot avoid wondering who we are, why we are talking in english in this popular square.</t>
+  </si>
+  <si>
     <t xml:space="preserve">V: Alright, let start then. </t>
   </si>
   <si>
@@ -82,11 +88,17 @@
     <t>V: Let me brifly interrupt you there, you mentioned the square was founded by Lorenzo Figueróa, but the name of the square has the name of a general. Who was San Martín?</t>
   </si>
   <si>
+    <t>SCENE 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">At this time, both start walking away from intial location towards San Martín's monument. 
 </t>
   </si>
   <si>
     <t xml:space="preserve">TG: San Martín was an Argentine general and the prime leader of the southern part of South America's successful struggle for independence from the Spanish Empire. He is a national hero and together with Simón Bolivar he is one of the Liberators of Spanish South America. The square exists since 1581 but since 1916 the monument you can see here was added. From that day on, the square carries his name. It is typical in Argentina that the main square in every major city has the general's name. </t>
+  </si>
+  <si>
+    <t>Next to the monument there are a lot of pigeons near some elder people sat in the seats near the trees. You can hear the first peddlers waking around the area.</t>
   </si>
   <si>
     <t xml:space="preserve">EXPERIENCE DETAIL: At this moment, if the viewer points the pointer towards San Martín's monument and click in it, the visitor should be able to see a close up of the moment with more details about them. </t>
@@ -98,7 +110,16 @@
     <t xml:space="preserve">TG: Ok, let's now go to the Cathedral. </t>
   </si>
   <si>
-    <t xml:space="preserve">At this moment, both now walk towards the main entrance of the Cathedral. </t>
+    <t>SCENE 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At this moment, both now walk towards the main entrance of the Cathedral. Here you can observe the drawing in the floor that mirrors the façade. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">At all times, there are peatons walking around us. They do not stop nor pay attention to what we are doing. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cars and Buses passes in the street next to the cathedral making the typical noises of a street with heavy traffic. </t>
   </si>
   <si>
     <t xml:space="preserve">TG: Ok, we are now in front of the Cathedral. Its construction was started in 1582 under the name of “Iglesia de Nuestra Señora de la Asunción”. It is built with stones, bricks and sand lime. The building was officially sacred in 1706. The existing façade was designed and conclude by Andrés Bianqui in 1729. The two main bell towers were concluded 1787. The main entrance as you can see it now was made by jesuits while there were here in Córdoba. During 1900 and 1914 a famous architect and painter added a few frescos to the vault. During the tour, the tour guide will elaborate on these concepts and more. The building was built in different periods and you can easily observe that fact. 
@@ -117,7 +138,10 @@
     <t xml:space="preserve">V: Really? </t>
   </si>
   <si>
-    <t xml:space="preserve">The visitor is very interested in all the architectural details the tour guide is explaining and showing. </t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>The visitor is very interested in all the architectural details the tour guide is explaining and showing.</t>
   </si>
   <si>
     <t xml:space="preserve">TG: Yes, but luckily for the workers, nobody die in those circunstances. </t>
@@ -132,14 +156,26 @@
     <t>V: Sure</t>
   </si>
   <si>
+    <t>SCENE 4</t>
+  </si>
+  <si>
     <t xml:space="preserve">At this moment, they approaches the front door. </t>
+  </si>
+  <si>
+    <t>There are individuals entering and leaving the cathedral at all times.</t>
   </si>
   <si>
     <t xml:space="preserve">TG: Ok, now we are going to talk about the atrium and the porch. </t>
   </si>
   <si>
+    <t>There is a police man next to the main entrance.</t>
+  </si>
+  <si>
     <t>TG:Formerly the atrium was closed by pillars and bars, which then removed. In 1878, the three gates forged by the craftsman Fidel Massa, in his smithy "Horse" were placed. In the main, the apostles St. Peter and St. Paul and above the stated date. On the side, at the top, "Mary" and "Joseph" reads, respectively.
 The cancel input, wooden missions belonged to the church of the Society of Jesus, until the expulsion of the order in 1767. The doors, carob, are adorned with studs and stylized figures callers.</t>
+  </si>
+  <si>
+    <t>While the TG is talking about Dean Funes, 2 women enter the same area and start looking at the monument behind us.</t>
   </si>
   <si>
     <t xml:space="preserve">EXPERIENCE DETAIL: At this point, the viewer can do the close ups for the atrium, urn under the porch and the monuments of José María Paz and his wife. </t>
@@ -154,6 +190,9 @@
     <t xml:space="preserve">V: And what about now the monuments in the other side. </t>
   </si>
   <si>
+    <t>At this time as we approarches, the two women move to Dean Funes' monument. They pass next to us without paying attention to us.</t>
+  </si>
+  <si>
     <t>TG: In another monument, the work of De la Cárcova, the embalmed body of Gral. José María Paz and the remains of his wife Margarita. Peace participated in the wars of Independence and Brazil. Also in our civil strife.</t>
   </si>
   <si>
@@ -163,10 +202,22 @@
     <t xml:space="preserve">V: Sure. Can't wait. </t>
   </si>
   <si>
+    <t>SCENE 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">They now enter the Cathedral. </t>
   </si>
   <si>
+    <t>Music with very low volume sounds in background.</t>
+  </si>
+  <si>
     <t xml:space="preserve">TG: At this point, we will talk about the different chapels inside the Cathedral. </t>
+  </si>
+  <si>
+    <t>There are different people sat in different rows. Some are in silence, some others are talking between each other.</t>
+  </si>
+  <si>
+    <t>There is no ongoing celebrations at the time we enter the cathedral.</t>
   </si>
   <si>
     <t>V: How many chapels exists inside this cathedral?</t>
@@ -228,6 +279,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">When we enter this chapel, there is a man next to the image of Nuestra Señora de Nieva reading the tourist information about her. This man stays there for a few minutes and then leave this chapel. </t>
+  </si>
+  <si>
     <t>TG: The altarpiece for "Nuestra Señora de Niva" and decoration, belongs to Manuel Garay, who led the Innocent carpenter in construction. An anonymous sculptor modeled the two angels placed in the attic. It is composed of columns and Corinthian columns, closing a space crowned by an inner dome.
 Reredos and image were blessed by Bishop Moscoso, on October 19, 1797, who had ruled that "the second Sunday of November is celebrated the feast of" Our Lady of the Soterraña de Nieva ".</t>
   </si>
@@ -242,34 +296,22 @@
     <t>V: Ok, now what's next?</t>
   </si>
   <si>
-    <t>TG: We are going to Cabildo now</t>
+    <t>SCENE 6</t>
   </si>
   <si>
-    <t>At this point, the visitor and tour guide walks out the cathedral and moves to Cabildo main entrance.</t>
+    <t>TG: We are going to Cabildo now. Both the TG and visitor walk towards cabildo and enter the main door.</t>
   </si>
   <si>
-    <t xml:space="preserve">TG: Ok, we are now at Cabildo. At this location we will visit Patio Mayor, Patio Menor and the prison </t>
+    <t xml:space="preserve">There are three policemen inside cabildo talking between each other. There is another person sat on a desk with touristik information. </t>
   </si>
   <si>
-    <t xml:space="preserve">There are some police man talking between each other at the entrance of the building. </t>
+    <t xml:space="preserve">At this time of the day, there is a lot of noise outside in the main square, cars, buses, some people talking loud, etc. </t>
   </si>
   <si>
-    <t>TG: The local government in Córdoba met in its members' private homes in the first years after the settlement's 1573 establishment. The first structure designated for the purpose was begun in 1588, and was a modest adobe and thatched roof structure typical of the colonial era in Spanish America. A framed wood structure designed by Alonso de Encinas replaced the precarious, initial cabildo in 1610.</t>
+    <t xml:space="preserve">TG: As you can see it now, in this building we had the house of the governor, the city hall and the prision. This building was similar to other Cabildos across the country. </t>
   </si>
   <si>
-    <t xml:space="preserve">TG: Encinas' cabildo, which included only the Alcalde's office, living quarters and a small jail, was ordered replaced by a larger building in 1749 by the Alcade (Mayor), José Moyano Oscariz. The Governor of Córdoba appointed in 1783, the Marquess of Sobremonte, Rafael Núñez, prioritized the much delayed completion of the new Cabildo. He commissioned Juan Manuel López for the new project, which would feature a significantly larger office space, grand steps, a chapel, a patio, an archway of fifteen columns along the façade, and a covered arcade along the archway for the inclusion of storefronts. The greatly accelerated works were concluded in 1786, and would include the opening of the Santa Catalina Promenade between the cabildo and the recently built Córdoba Cathedral.
-Marble cladding and a bell tower were added in 1885, though the latter was removed during the cabildo's restoration in the late 1930s, when numerous historic structures in Argentina were restored to their approximate, original design by having such additions demolished. The Córdoba Cabildo, like the Cathedral, was declared a National Historic Monument in 1941. The city government was relocated to a Renaissance Revivalist structure late in the 19th century, and to a Modernist building (its current home) in the 1960s. A section of the historic cabildo remained in use by the Provincial Police Department of Information (DDI), however, and during the last dictatorship, this wing was used as one of over 300 detention centers operated by the regime during the Dirty War of the late 1970s.
-he City Historical Museum was inaugurated at the cabildo in 1980.
-</t>
-  </si>
-  <si>
-    <t>TG: Let's now move to the interior of Cabildo</t>
-  </si>
-  <si>
-    <t>V: OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TG: On the left side of the building we have the main part of the building, this was around the main patio or patio mayor. As you can see it now, in this building we had the house of the governor, the city hall and the prision. This building was similar to other Cabildos across the country. </t>
+    <t>There are other visitors in patio mayor reading the information that is hanging in the walls.</t>
   </si>
   <si>
     <t>EXPERIENCE DETAILS. The viewer can position the experience in the patio center and click on the different architecture elements to learn more about them.</t>
@@ -287,10 +329,16 @@
     <t>TG: No, we can only see them from outside. We will now go to the next patio.</t>
   </si>
   <si>
+    <t>SCENE 7</t>
+  </si>
+  <si>
     <t xml:space="preserve">At this point. TG and Visitor moves to the other patio: Patio Menor. </t>
   </si>
   <si>
     <t xml:space="preserve">TG: On this side of the building we have a similar, but smaller, structure of the building and as you can observe there is an interesting discovery that accidentally happened in 2016. </t>
+  </si>
+  <si>
+    <t>There are other tourists also watching the new discovery with another tour guide explaining the same information. This conversion is happening in spanish language.</t>
   </si>
   <si>
     <t>V: What was that?</t>
@@ -320,7 +368,13 @@
     <t>V: Alright</t>
   </si>
   <si>
+    <t>SCENE 8</t>
+  </si>
+  <si>
     <t xml:space="preserve">At this point, TG and visitor goes 1 floor underground. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When we enter the cells there is a woman reading the touristic information.  </t>
   </si>
   <si>
     <t>TG: We are now underground. You can observe now that we have 2 different floor levels.</t>
@@ -344,6 +398,9 @@
     <t>At this time, the tour guide shows the space available for prisioners in the cells.</t>
   </si>
   <si>
+    <t xml:space="preserve">While I'm observing the vertical space available for prisioners the woman that was there when we arrive leaves the room. </t>
+  </si>
+  <si>
     <t>V: Until which year this was used as a prision?</t>
   </si>
   <si>
@@ -362,6 +419,9 @@
     <t xml:space="preserve">TG: This was not a room at that time. It was the watering system and was not directly connected to the cells. It was just next to it but completely sealed. </t>
   </si>
   <si>
+    <t xml:space="preserve">At this time, the same tourists that were before in patio menor comes to see the prision. </t>
+  </si>
+  <si>
     <t xml:space="preserve">EXPERIENCE DETAILS: When the user selects the poster explaining the watering system the poster turns into an animation that present how the watering system works. </t>
   </si>
   <si>
@@ -374,7 +434,13 @@
     <t>V: Alright.</t>
   </si>
   <si>
+    <t>SCENE 9</t>
+  </si>
+  <si>
     <t xml:space="preserve">At this moment, both TG and V goes out of Cabildo to wrap up the tour. </t>
+  </si>
+  <si>
+    <t>The square and the front of cabildo is very crowded. There are a lot of people passing by since it is almost midday</t>
   </si>
   <si>
     <t xml:space="preserve">TG: OK, with this we have covered our last location and this conclude our tour to Centro Histórico.  </t>
@@ -391,12 +457,21 @@
   <si>
     <t xml:space="preserve">At this point the guide and visitor shake hands and goes into different ways. The scene turns blurry and fades out into a black screen where the credits will be presented. </t>
   </si>
+  <si>
+    <t xml:space="preserve">REFERENCES: </t>
+  </si>
+  <si>
+    <t>Details for the interactive scenes.</t>
+  </si>
+  <si>
+    <t>Change the scene.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -407,12 +482,16 @@
     </font>
     <font/>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,8 +506,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
         <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -443,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -462,12 +553,36 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,14 +881,14 @@
       <c r="Y9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -798,11 +913,9 @@
     </row>
     <row r="11">
       <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -827,9 +940,11 @@
     </row>
     <row r="12">
       <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -883,9 +998,7 @@
     </row>
     <row r="14">
       <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -913,7 +1026,7 @@
     <row r="15">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -942,9 +1055,11 @@
     <row r="16">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -999,7 +1114,9 @@
     </row>
     <row r="18">
       <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1026,12 +1143,12 @@
     </row>
     <row r="19">
       <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1055,13 +1172,9 @@
     </row>
     <row r="20">
       <c r="A20" s="3"/>
-      <c r="B20" s="4" t="s">
-        <v>24</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1085,13 +1198,14 @@
       <c r="Y20" s="3"/>
     </row>
     <row r="21">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
+      <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -1118,8 +1232,12 @@
       <c r="B22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1144,11 +1262,11 @@
     </row>
     <row r="23">
       <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1174,12 +1292,10 @@
     <row r="24">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1202,13 +1318,19 @@
       <c r="X24" s="3"/>
       <c r="Y24" s="3"/>
     </row>
-    <row r="25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
-        <v>31</v>
+    <row r="25" ht="31.5" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>32</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="B25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1234,10 +1356,11 @@
     <row r="26">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1263,12 +1386,10 @@
     <row r="27">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1294,7 +1415,7 @@
     <row r="28">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1323,10 +1444,12 @@
     <row r="29">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="D29" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1352,7 +1475,7 @@
     <row r="30">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -1381,7 +1504,7 @@
     <row r="31">
       <c r="A31" s="3"/>
       <c r="B31" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1409,11 +1532,11 @@
     </row>
     <row r="32">
       <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
+      <c r="B32" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="4" t="s">
-        <v>39</v>
-      </c>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
@@ -1438,7 +1561,9 @@
     </row>
     <row r="33">
       <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
+      <c r="B33" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1466,7 +1591,7 @@
     <row r="34">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1493,13 +1618,14 @@
       <c r="Y34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4" t="s">
-        <v>41</v>
+      <c r="A35" s="4" t="s">
+        <v>47</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="7" t="s">
-        <v>42</v>
+      <c r="B35" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
@@ -1525,10 +1651,9 @@
     </row>
     <row r="36">
       <c r="A36" s="3"/>
-      <c r="B36" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
@@ -1554,9 +1679,12 @@
     <row r="37">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -1582,9 +1710,14 @@
     <row r="38">
       <c r="A38" s="3"/>
       <c r="B38" s="4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
@@ -1610,7 +1743,7 @@
     <row r="39">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C39" s="3"/>
       <c r="E39" s="3"/>
@@ -1638,7 +1771,7 @@
     <row r="40">
       <c r="A40" s="3"/>
       <c r="B40" s="4" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C40" s="3"/>
       <c r="E40" s="3"/>
@@ -1666,9 +1799,11 @@
     <row r="41">
       <c r="A41" s="3"/>
       <c r="B41" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -1693,11 +1828,10 @@
     </row>
     <row r="42">
       <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
+      <c r="B42" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -1722,9 +1856,10 @@
     </row>
     <row r="43">
       <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
+      <c r="B43" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -1750,10 +1885,9 @@
     <row r="44">
       <c r="A44" s="3"/>
       <c r="B44" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -1776,13 +1910,17 @@
       <c r="X44" s="3"/>
       <c r="Y44" s="3"/>
     </row>
-    <row r="45">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4" t="s">
-        <v>51</v>
+    <row r="45" ht="26.25" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>62</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="B45" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="12"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -1808,11 +1946,13 @@
     <row r="46">
       <c r="A46" s="3"/>
       <c r="B46" s="4" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="7" t="s">
-        <v>53</v>
+      <c r="C46" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -1839,10 +1979,10 @@
     <row r="47">
       <c r="A47" s="3"/>
       <c r="B47" s="4" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -1868,10 +2008,12 @@
     <row r="48">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -1897,10 +2039,10 @@
     <row r="49">
       <c r="A49" s="3"/>
       <c r="B49" s="4" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="4"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -1926,7 +2068,7 @@
     <row r="50">
       <c r="A50" s="3"/>
       <c r="B50" s="4" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -1955,7 +2097,7 @@
     <row r="51">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -1984,9 +2126,11 @@
     <row r="52">
       <c r="A52" s="3"/>
       <c r="B52" s="4" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -2012,7 +2156,9 @@
     </row>
     <row r="53">
       <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
+      <c r="B53" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -2040,7 +2186,7 @@
     <row r="54">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2068,9 +2214,7 @@
     </row>
     <row r="55">
       <c r="A55" s="3"/>
-      <c r="B55" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -2098,7 +2242,7 @@
     <row r="56">
       <c r="A56" s="3"/>
       <c r="B56" s="4" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -2126,11 +2270,11 @@
     </row>
     <row r="57">
       <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="B57" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C57" s="3"/>
-      <c r="D57" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="D57" s="3"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2154,14 +2298,18 @@
       <c r="Y57" s="3"/>
     </row>
     <row r="58">
-      <c r="A58" s="3"/>
-      <c r="B58" s="4" t="s">
-        <v>64</v>
+      <c r="A58" s="4" t="s">
+        <v>80</v>
       </c>
-      <c r="C58" s="4" t="s">
-        <v>65</v>
+      <c r="B58" s="8" t="s">
+        <v>81</v>
       </c>
-      <c r="D58" s="4"/>
+      <c r="C58" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>83</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2186,13 +2334,9 @@
     </row>
     <row r="59">
       <c r="A59" s="3"/>
-      <c r="B59" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="B59" s="4"/>
       <c r="C59" s="3"/>
-      <c r="D59" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -2218,10 +2362,14 @@
     <row r="60">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="C60" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>86</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -2247,7 +2395,7 @@
     <row r="61">
       <c r="A61" s="3"/>
       <c r="B61" s="4" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2276,7 +2424,7 @@
     <row r="62">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -2305,12 +2453,10 @@
     <row r="63">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C63" s="3"/>
-      <c r="D63" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -2336,7 +2482,7 @@
     <row r="64">
       <c r="A64" s="3"/>
       <c r="B64" s="4" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -2362,13 +2508,14 @@
       <c r="X64" s="3"/>
       <c r="Y64" s="3"/>
     </row>
-    <row r="65">
-      <c r="A65" s="3"/>
-      <c r="B65" s="4" t="s">
-        <v>73</v>
+    <row r="65" ht="35.25" customHeight="1">
+      <c r="A65" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -2394,9 +2541,11 @@
     <row r="66">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="C66" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -2423,7 +2572,7 @@
     <row r="67">
       <c r="A67" s="3"/>
       <c r="B67" s="4" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -2451,10 +2600,12 @@
     </row>
     <row r="68">
       <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
+      <c r="B68" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="4" t="s">
-        <v>76</v>
+      <c r="D68" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -2481,7 +2632,7 @@
     <row r="69">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -2510,7 +2661,7 @@
     <row r="70">
       <c r="A70" s="3"/>
       <c r="B70" s="4" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -2539,12 +2690,10 @@
     <row r="71">
       <c r="A71" s="3"/>
       <c r="B71" s="4" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="7" t="s">
-        <v>80</v>
-      </c>
+      <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -2570,7 +2719,7 @@
     <row r="72">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -2598,9 +2747,7 @@
     </row>
     <row r="73">
       <c r="A73" s="3"/>
-      <c r="B73" s="4" t="s">
-        <v>82</v>
-      </c>
+      <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -2628,7 +2775,7 @@
     <row r="74">
       <c r="A74" s="3"/>
       <c r="B74" s="4" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -2657,7 +2804,7 @@
     <row r="75">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -2683,11 +2830,16 @@
       <c r="X75" s="3"/>
       <c r="Y75" s="3"/>
     </row>
-    <row r="76">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
+    <row r="76" ht="36.0" customHeight="1">
+      <c r="A76" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -2713,10 +2865,12 @@
     <row r="77">
       <c r="A77" s="3"/>
       <c r="B77" s="4" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -2742,7 +2896,7 @@
     <row r="78">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -2770,10 +2924,11 @@
     </row>
     <row r="79">
       <c r="A79" s="3"/>
+      <c r="B79" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="C79" s="3"/>
-      <c r="D79" s="4" t="s">
-        <v>87</v>
-      </c>
+      <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -2799,12 +2954,10 @@
     <row r="80">
       <c r="A80" s="3"/>
       <c r="B80" s="4" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="C80" s="3"/>
-      <c r="D80" s="7" t="s">
-        <v>89</v>
-      </c>
+      <c r="D80" s="3"/>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -2830,7 +2983,7 @@
     <row r="81">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
@@ -2859,10 +3012,11 @@
     <row r="82">
       <c r="A82" s="3"/>
       <c r="B82" s="4" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
-      <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="C82" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -2888,7 +3042,7 @@
     <row r="83">
       <c r="A83" s="3"/>
       <c r="B83" s="4" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -2917,7 +3071,7 @@
     <row r="84">
       <c r="A84" s="3"/>
       <c r="B84" s="4" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -2945,11 +3099,11 @@
     </row>
     <row r="85">
       <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
+      <c r="B85" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="C85" s="3"/>
-      <c r="D85" s="4" t="s">
-        <v>94</v>
-      </c>
+      <c r="D85" s="3"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -2974,9 +3128,7 @@
     </row>
     <row r="86">
       <c r="A86" s="3"/>
-      <c r="B86" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3004,7 +3156,7 @@
     <row r="87">
       <c r="A87" s="3"/>
       <c r="B87" s="4" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -3033,7 +3185,7 @@
     <row r="88">
       <c r="A88" s="3"/>
       <c r="B88" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -3061,9 +3213,15 @@
     </row>
     <row r="89">
       <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="B89" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -3088,8 +3246,8 @@
     </row>
     <row r="90">
       <c r="A90" s="3"/>
-      <c r="B90" s="4" t="s">
-        <v>98</v>
+      <c r="B90" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -3118,7 +3276,7 @@
     <row r="91">
       <c r="A91" s="3"/>
       <c r="B91" s="4" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -3147,12 +3305,10 @@
     <row r="92">
       <c r="A92" s="3"/>
       <c r="B92" s="4" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="7" t="s">
-        <v>101</v>
-      </c>
+      <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -3175,13 +3331,16 @@
       <c r="X92" s="3"/>
       <c r="Y92" s="3"/>
     </row>
-    <row r="93">
-      <c r="A93" s="3"/>
+    <row r="93" ht="27.75" customHeight="1">
+      <c r="A93" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="B93" s="8" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
-      <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="C93" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -3207,7 +3366,7 @@
     <row r="94">
       <c r="A94" s="3"/>
       <c r="B94" s="4" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -3236,7 +3395,7 @@
     <row r="95">
       <c r="A95" s="3"/>
       <c r="B95" s="4" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
@@ -3264,11 +3423,10 @@
     </row>
     <row r="96">
       <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
+      <c r="B96" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C96" s="3"/>
-      <c r="D96" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -3294,7 +3452,7 @@
     <row r="97">
       <c r="A97" s="3"/>
       <c r="B97" s="4" t="s">
-        <v>106</v>
+        <v>132</v>
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
@@ -3322,11 +3480,10 @@
     </row>
     <row r="98">
       <c r="A98" s="3"/>
-      <c r="B98" s="4" t="s">
-        <v>107</v>
+      <c r="B98" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
@@ -3351,10 +3508,9 @@
     </row>
     <row r="99">
       <c r="A99" s="3"/>
-      <c r="B99" s="4" t="s">
-        <v>108</v>
-      </c>
+      <c r="B99" s="3"/>
       <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
@@ -3379,9 +3535,7 @@
     </row>
     <row r="100">
       <c r="A100" s="3"/>
-      <c r="B100" s="4" t="s">
-        <v>109</v>
-      </c>
+      <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -3407,12 +3561,12 @@
       <c r="Y100" s="3"/>
     </row>
     <row r="101">
-      <c r="A101" s="3"/>
+      <c r="A101" s="4" t="s">
+        <v>134</v>
+      </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="4" t="s">
-        <v>110</v>
-      </c>
+      <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
@@ -3436,8 +3590,10 @@
       <c r="Y101" s="3"/>
     </row>
     <row r="102">
-      <c r="A102" s="3"/>
-      <c r="B102" s="3"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -3463,8 +3619,10 @@
       <c r="Y102" s="3"/>
     </row>
     <row r="103">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
+      <c r="A103" s="15"/>
+      <c r="B103" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
@@ -27708,90 +27866,9 @@
       <c r="X1000" s="3"/>
       <c r="Y1000" s="3"/>
     </row>
-    <row r="1001">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="3"/>
-      <c r="D1001" s="3"/>
-      <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="3"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="3"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="3"/>
-      <c r="O1001" s="3"/>
-      <c r="P1001" s="3"/>
-      <c r="Q1001" s="3"/>
-      <c r="R1001" s="3"/>
-      <c r="S1001" s="3"/>
-      <c r="T1001" s="3"/>
-      <c r="U1001" s="3"/>
-      <c r="V1001" s="3"/>
-      <c r="W1001" s="3"/>
-      <c r="X1001" s="3"/>
-      <c r="Y1001" s="3"/>
-    </row>
-    <row r="1002">
-      <c r="A1002" s="3"/>
-      <c r="B1002" s="3"/>
-      <c r="C1002" s="3"/>
-      <c r="D1002" s="3"/>
-      <c r="E1002" s="3"/>
-      <c r="F1002" s="3"/>
-      <c r="G1002" s="3"/>
-      <c r="H1002" s="3"/>
-      <c r="I1002" s="3"/>
-      <c r="J1002" s="3"/>
-      <c r="K1002" s="3"/>
-      <c r="L1002" s="3"/>
-      <c r="M1002" s="3"/>
-      <c r="N1002" s="3"/>
-      <c r="O1002" s="3"/>
-      <c r="P1002" s="3"/>
-      <c r="Q1002" s="3"/>
-      <c r="R1002" s="3"/>
-      <c r="S1002" s="3"/>
-      <c r="T1002" s="3"/>
-      <c r="U1002" s="3"/>
-      <c r="V1002" s="3"/>
-      <c r="W1002" s="3"/>
-      <c r="X1002" s="3"/>
-      <c r="Y1002" s="3"/>
-    </row>
-    <row r="1003">
-      <c r="A1003" s="3"/>
-      <c r="B1003" s="3"/>
-      <c r="C1003" s="3"/>
-      <c r="D1003" s="3"/>
-      <c r="E1003" s="3"/>
-      <c r="F1003" s="3"/>
-      <c r="G1003" s="3"/>
-      <c r="H1003" s="3"/>
-      <c r="I1003" s="3"/>
-      <c r="J1003" s="3"/>
-      <c r="K1003" s="3"/>
-      <c r="L1003" s="3"/>
-      <c r="M1003" s="3"/>
-      <c r="N1003" s="3"/>
-      <c r="O1003" s="3"/>
-      <c r="P1003" s="3"/>
-      <c r="Q1003" s="3"/>
-      <c r="R1003" s="3"/>
-      <c r="S1003" s="3"/>
-      <c r="T1003" s="3"/>
-      <c r="U1003" s="3"/>
-      <c r="V1003" s="3"/>
-      <c r="W1003" s="3"/>
-      <c r="X1003" s="3"/>
-      <c r="Y1003" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D35:D41"/>
+    <mergeCell ref="D38:D44"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <drawing r:id="rId1"/>

</xml_diff>